<commit_message>
test with new CPLEX parameters
</commit_message>
<xml_diff>
--- a/Instances/G0041442b2_NonStationary.xlsx
+++ b/Instances/G0041442b2_NonStationary.xlsx
@@ -986,20 +986,20 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0016</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>35</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0032</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
         <v>49</v>
       </c>
       <c r="H2" t="s"/>
       <c r="I2" t="n">
-        <v>0.032</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1013,20 +1013,20 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0028</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
         <v>15</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0056</v>
+        <v>14</v>
       </c>
       <c r="G3" t="n">
         <v>21</v>
       </c>
       <c r="H3" t="s"/>
       <c r="I3" t="n">
-        <v>0.056</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1040,20 +1040,20 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0024</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
         <v>25</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0048</v>
+        <v>12</v>
       </c>
       <c r="G4" t="n">
         <v>35</v>
       </c>
       <c r="H4" t="s"/>
       <c r="I4" t="n">
-        <v>0.048</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1067,20 +1067,20 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0012</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>50</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0024</v>
+        <v>6</v>
       </c>
       <c r="G5" t="n">
         <v>70</v>
       </c>
       <c r="H5" t="s"/>
       <c r="I5" t="n">
-        <v>0.024</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1094,20 +1094,20 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0012</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
         <v>200</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0024</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="s"/>
       <c r="I6" t="n">
-        <v>0.024</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1121,20 +1121,20 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0012</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
         <v>160</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0024</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="s"/>
       <c r="I7" t="n">
-        <v>0.024</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1148,20 +1148,20 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0008</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
         <v>300</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0016</v>
+        <v>4</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="s"/>
       <c r="I8" t="n">
-        <v>0.016</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1175,20 +1175,20 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0004</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>800</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0008</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="s"/>
       <c r="I9" t="n">
-        <v>0.008</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1202,20 +1202,20 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0004</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>1440</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0008</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="s"/>
       <c r="I10" t="n">
-        <v>0.008</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1229,20 +1229,20 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0004</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>1840</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0008</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="s"/>
       <c r="I11" t="n">
-        <v>0.008</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>